<commit_message>
work in summer 23
</commit_message>
<xml_diff>
--- a/Landers_DB23.xlsx
+++ b/Landers_DB23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Conall De Paor\Desktop\Supaero\Research Project\Sizing-Tool\ORLA_Lander_Mission_Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B99EF66-275D-4DC0-8CAF-F97BC5315830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68077180-9A68-4A0F-8801-E2EC36194C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" firstSheet="5" activeTab="5" xr2:uid="{00204FEE-323F-4DA1-86F4-8FD253E43B4D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00204FEE-323F-4DA1-86F4-8FD253E43B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="All Landers" sheetId="1" r:id="rId1"/>
@@ -4686,7 +4686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29D0D7DD-07B0-4637-A9ED-F61198FECE0D}" type="CELLRANGE">
+                    <a:fld id="{DFF20DCB-E6F3-447F-8C7F-11E036D3B343}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11383,9 +11383,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.15735870516185477"/>
-          <c:y val="5.0925925925925923E-2"/>
-          <c:w val="0.74646916010498687"/>
-          <c:h val="0.68889690871974341"/>
+          <c:y val="9.6054270139309506E-2"/>
+          <c:w val="0.67182318426412913"/>
+          <c:h val="0.64376854431657582"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -11751,6 +11751,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.27016305394258139"/>
+                  <c:y val="-7.9644013729053095E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Medium (analysis)'!$Q$2:$Q$32</c:f>
@@ -15795,6 +15845,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.7436329424120428E-2"/>
+                  <c:y val="-0.16967957130358705"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Large (analysis)'!$S$2:$S$18</c:f>
@@ -36091,12 +36192,12 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -40803,8 +40904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81822334-6E3E-4E3D-93CF-BF9B02F79F45}">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView topLeftCell="K23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U50" sqref="U50"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42107,7 +42208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D7CEE9-61DB-45C0-903D-6E17D60508FA}">
   <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -43367,8 +43468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BD2F64-B90E-43D4-AEE3-5B9F2B1E7FA0}">
   <dimension ref="A1:AH18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>